<commit_message>
Beginning replacement of mapping from procedure name to procedure group
</commit_message>
<xml_diff>
--- a/4-Construct/NotificationPlacingWayName_groupings.xlsx
+++ b/4-Construct/NotificationPlacingWayName_groupings.xlsx
@@ -26,18 +26,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Shaun McGirr</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Shaun McGirr:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Later recoded to "Type of procedure"</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
-  <si>
-    <t>Type of procedure</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>Freq</t>
   </si>
   <si>
-    <t>Procedure group</t>
-  </si>
-  <si>
     <t>Заказ на выполнение проектных, изыскательских работ, работ по строительству, реконструкции, капитальному ремонту объектов капитального строительства, относящихся в соответствии с Федеральным законом от 1 декабря 2007 года № 310-ФЗ к олимпийским объектам федерального значения, олимпийским объектам краевого значения или олимпийским объектам муниципального значения (ч.34 ст.65 Федерального закона №94-ФЗ), размещаемый путем проведения запроса котировок</t>
   </si>
   <si>
@@ -89,9 +115,6 @@
     <t>Open tender</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Higher discretion</t>
   </si>
   <si>
@@ -101,14 +124,35 @@
     <t>Medium discretion</t>
   </si>
   <si>
-    <t>Discretion</t>
+    <t>Предварительный отбор</t>
+  </si>
+  <si>
+    <t>Preliminary selection</t>
+  </si>
+  <si>
+    <t>Сообщение о заинтересованности в проведении открытого конкурса</t>
+  </si>
+  <si>
+    <t>Registration of interest in open tender</t>
+  </si>
+  <si>
+    <t>NotificationPlacingWayName</t>
+  </si>
+  <si>
+    <t>TenderProcedureGroup</t>
+  </si>
+  <si>
+    <t>TenderProcedureDiscretion</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -121,6 +165,17 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -518,8 +573,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -536,198 +591,226 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="78" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>21350</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>2727</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>222226</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B11">
+        <v>118191</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
         <v>211</v>
       </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12">
-        <v>118191</v>
-      </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="65" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>55</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -738,5 +821,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>